<commit_message>
changed port to 5432
</commit_message>
<xml_diff>
--- a/Resources/monthly_home_sales.xlsx
+++ b/Resources/monthly_home_sales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab74b0f1fe3ad570/Desktop/Challenges/Austin_Housing_Market/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab74b0f1fe3ad570/Desktop/Challenges/Final-Project-Austin-Housing-Market/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{2ADBE80D-74A6-428F-AB80-90B8300FDDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A83A632-6599-45A7-9712-F429C2681C17}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{2ADBE80D-74A6-428F-AB80-90B8300FDDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE71B75B-C227-499B-99CD-60B3226A1AAC}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5256" yWindow="396" windowWidth="24960" windowHeight="15288" xr2:uid="{10CE9F22-9622-4826-B65B-A329A3C5FEE1}"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{10CE9F22-9622-4826-B65B-A329A3C5FEE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,10 +171,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,14 +472,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006FD09B-0722-46E6-A5D0-FCBEED71FA87}">
   <dimension ref="A1:G401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
     <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" customWidth="1"/>
   </cols>

</xml_diff>